<commit_message>
Removed unwanted files and folder
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885A356C-5148-4CB5-91B2-6343D449FC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA068739-327D-4B02-ADE7-3D04BE49EFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{B6E74BE3-B2FD-48D1-A0D5-C37F8BDBF8FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>number</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Aysuhi</t>
+  </si>
+  <si>
+    <t>number1</t>
   </si>
 </sst>
 </file>
@@ -462,43 +465,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC19047-295F-453F-92D9-D3B5EB065FEF}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
         <v>8107308639</v>
       </c>
+      <c r="C2">
+        <v>7878776426</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>7357240129</v>
       </c>
+      <c r="C3">
+        <v>7357240129</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -506,7 +519,7 @@
         <v>8306405898</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -514,7 +527,7 @@
         <v>7850010081</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>

</xml_diff>